<commit_message>
hochladen der Erste version der Moter Ansteuerung + Aktualisierung der AZE im project_overview.xlsx file
</commit_message>
<xml_diff>
--- a/project_overview.xlsx
+++ b/project_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023-2024\ESY\self_driving_car\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794FAA3F-A30D-4648-92A1-6D551C641666}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D902F1F-E201-4D12-A994-F2E78168C807}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="228">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1114,6 +1114,12 @@
   </si>
   <si>
     <t>Einführung in Git hub, durch Prof. Jahn</t>
+  </si>
+  <si>
+    <t>Beschprechung (Informationen bzg. ESY Matura)</t>
+  </si>
+  <si>
+    <t>Kopieren des Beispielcodes aus dem Datasheet für den Motortreiber + Löten der stromversorgungen und befestigen des Batteriefach am Chasie</t>
   </si>
 </sst>
 </file>
@@ -1843,12 +1849,45 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1858,36 +1897,6 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1911,9 +1920,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2400,14 +2406,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="127" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2456,10 +2462,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="116"/>
+      <c r="F7" s="122"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2470,8 +2476,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2482,8 +2488,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2494,8 +2500,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2506,8 +2512,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2528,49 +2534,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="121"/>
-      <c r="C15" s="121"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="121"/>
-      <c r="F15" s="121"/>
+      <c r="B15" s="125"/>
+      <c r="C15" s="125"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="125"/>
+      <c r="F15" s="125"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="122"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
-      <c r="F16" s="122"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="122"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="122"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="127"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2583,64 +2589,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="128" t="s">
+      <c r="A23" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="128"/>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="121"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116" t="s">
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="124" t="s">
+      <c r="A27" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="124"/>
-      <c r="C27" s="124"/>
-      <c r="D27" s="129"/>
-      <c r="E27" s="129"/>
-      <c r="F27" s="129"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="123" t="s">
+      <c r="A28" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="123"/>
-      <c r="C28" s="123"/>
-      <c r="D28" s="124" t="s">
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="117" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="125" t="s">
+      <c r="A29" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="125"/>
-      <c r="C29" s="125"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="126"/>
-      <c r="F29" s="126"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2651,16 +2667,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2734,29 +2740,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="130"/>
+      <c r="C3" s="131"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="130"/>
+      <c r="C4" s="131"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="130" t="s">
+      <c r="B5" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="130"/>
+      <c r="C5" s="131"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2979,11 +2985,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -2991,18 +2997,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="133" t="s">
+      <c r="A4" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="134"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -3270,14 +3276,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3570,16 +3576,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="127" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4212,19 +4218,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -4888,16 +4894,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -5673,71 +5679,71 @@
       <c r="A21" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="137" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="136"/>
-      <c r="D21" s="136"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="137" t="s">
+      <c r="B22" s="138" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="137"/>
-      <c r="D22" s="137"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="137" t="s">
+      <c r="B23" s="138" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="137"/>
-      <c r="D23" s="137"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="137" t="s">
+      <c r="B24" s="138" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="135"/>
-      <c r="C25" s="135"/>
-      <c r="D25" s="135"/>
+      <c r="B25" s="136"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="136"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="135"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="135"/>
+      <c r="B26" s="136"/>
+      <c r="C26" s="136"/>
+      <c r="D26" s="136"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="135"/>
-      <c r="D27" s="135"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="136"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="135"/>
-      <c r="C28" s="135"/>
-      <c r="D28" s="135"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="136"/>
+      <c r="D28" s="136"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="135"/>
-      <c r="C29" s="135"/>
-      <c r="D29" s="135"/>
+      <c r="B29" s="136"/>
+      <c r="C29" s="136"/>
+      <c r="D29" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5775,7 +5781,7 @@
   <dimension ref="A1:AMO33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,16 +5797,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5869,7 +5875,7 @@
       <c r="F5" s="85" t="s">
         <v>223</v>
       </c>
-      <c r="G5" s="138">
+      <c r="G5" s="115">
         <v>0.7</v>
       </c>
       <c r="H5" s="85"/>
@@ -5927,21 +5933,43 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="85"/>
+      <c r="A8" s="40">
+        <v>45257</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="111">
+        <v>0.5625</v>
+      </c>
+      <c r="D8" s="111">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="E8" s="105" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>47</v>
+      </c>
       <c r="G8" s="105"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="105"/>
+    <row r="9" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>45257</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="111">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D9" s="111">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="E9" s="105" t="s">
+        <v>227</v>
+      </c>
       <c r="F9" s="85"/>
       <c r="G9" s="105"/>
       <c r="H9" s="2"/>

</xml_diff>

<commit_message>
updaten AZE in project_overview.xlsx + umbennenung der moter_ansteuerung_v0.1 in moter_ansteuerung + updaten moter_ansteuerung auf v_1.0
</commit_message>
<xml_diff>
--- a/project_overview.xlsx
+++ b/project_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023-2024\ESY\self_driving_car\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023-2024\ESY\self_driving_car\reposi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D902F1F-E201-4D12-A994-F2E78168C807}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F97BEB-6EFC-4D66-8D5D-1CE18713439B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="233">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1101,15 +1101,9 @@
     <t xml:space="preserve">Zeitplan definieren, Stunden Abschätzen, Arbeitstagebuch </t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>wechseln der oberen platte, befestigen des motorschilds auf der unteren Platte, suchen einer geeigneten Beilagscheibe zum bestigen des motorschildes (nicht gefunden), entweder weitersuchen oder neue Löcher Bohren</t>
   </si>
   <si>
-    <t>2.1</t>
-  </si>
-  <si>
     <t>Krank</t>
   </si>
   <si>
@@ -1120,6 +1114,27 @@
   </si>
   <si>
     <t>Kopieren des Beispielcodes aus dem Datasheet für den Motortreiber + Löten der stromversorgungen und befestigen des Batteriefach am Chasie</t>
+  </si>
+  <si>
+    <t>Ausfüllen der AZE</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>Erste Inbetriebnahme der motoren mittels HIGH/LOW und Implementierung des Start/Stop-taster + Verkabelung Selbiger</t>
+  </si>
+  <si>
+    <t>2-3, 2-4</t>
+  </si>
+  <si>
+    <t>100%, 60%</t>
+  </si>
+  <si>
+    <t>2-3, 2-1</t>
   </si>
 </sst>
 </file>
@@ -1852,6 +1867,30 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1870,32 +1909,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2406,14 +2421,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2462,10 +2477,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="122" t="s">
+      <c r="E7" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="122"/>
+      <c r="F7" s="117"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2476,8 +2491,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2488,8 +2503,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2500,8 +2515,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2512,8 +2527,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="124"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2534,49 +2549,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="126"/>
-      <c r="C16" s="126"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
+      <c r="B16" s="123"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="126"/>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="126"/>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
+      <c r="B18" s="123"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="120"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2589,74 +2604,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="121"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="122" t="s">
+      <c r="A26" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="122"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122" t="s">
+      <c r="B26" s="117"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
+      <c r="B27" s="125"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117" t="s">
+      <c r="B28" s="124"/>
+      <c r="C28" s="124"/>
+      <c r="D28" s="125" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="125"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="118"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2667,6 +2672,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2740,11 +2755,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="131" t="s">
@@ -3562,7 +3577,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3576,16 +3591,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5781,7 +5796,7 @@
   <dimension ref="A1:AMO33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5851,9 +5866,11 @@
         <v>220</v>
       </c>
       <c r="F4" s="114" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="107"/>
+        <v>227</v>
+      </c>
+      <c r="G4" s="107" t="s">
+        <v>47</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5870,10 +5887,10 @@
         <v>0.6743055555555556</v>
       </c>
       <c r="E5" s="105" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5" s="85" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="G5" s="115">
         <v>0.7</v>
@@ -5896,7 +5913,7 @@
         <v>-</v>
       </c>
       <c r="E6" s="105" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F6" s="85" t="s">
         <v>47</v>
@@ -5922,7 +5939,7 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="E7" s="105" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F7" s="85" t="s">
         <v>47</v>
@@ -5946,12 +5963,14 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="E8" s="105" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F8" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="105"/>
+      <c r="G8" s="105" t="s">
+        <v>47</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5968,34 +5987,64 @@
         <v>0.67361111111111116</v>
       </c>
       <c r="E9" s="105" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="85"/>
+        <v>225</v>
+      </c>
+      <c r="F9" s="85" t="s">
+        <v>232</v>
+      </c>
       <c r="G9" s="105"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="105"/>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>45264</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="111">
+        <v>0.5625</v>
+      </c>
+      <c r="D10" s="111">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E10" s="105" t="s">
+        <v>229</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" s="115" t="s">
+        <v>231</v>
+      </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="105"/>
+      <c r="A11" s="40">
+        <v>45264</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="111">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D11" s="111">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>227</v>
+      </c>
+      <c r="G11" s="105" t="s">
+        <v>47</v>
+      </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="41"/>
       <c r="C12" s="111"/>
       <c r="D12" s="111"/>
@@ -6005,7 +6054,7 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="41"/>
       <c r="C13" s="111"/>
       <c r="D13" s="111"/>
@@ -6015,7 +6064,7 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="41"/>
       <c r="C14" s="111"/>
       <c r="D14" s="111"/>
@@ -6025,7 +6074,7 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="41"/>
       <c r="C15" s="111"/>
       <c r="D15" s="111"/>
@@ -6035,7 +6084,6 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
       <c r="B16" s="41"/>
       <c r="C16" s="111"/>
       <c r="D16" s="111"/>
@@ -6045,7 +6093,7 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="41"/>
       <c r="C17" s="111"/>
       <c r="D17" s="111"/>
@@ -6055,7 +6103,7 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="41"/>
       <c r="C18" s="111"/>
       <c r="D18" s="111"/>

</xml_diff>

<commit_message>
Update der AZE in project_overview.xlsx + Update der moter_ansteuerung (Sensor Wert beeinflusst PWM-Signal)
</commit_message>
<xml_diff>
--- a/project_overview.xlsx
+++ b/project_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023-2024\ESY\self_driving_car\reposi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F97BEB-6EFC-4D66-8D5D-1CE18713439B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E72D9B9-E2E4-454E-A507-3FAE298D956F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="236">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1135,6 +1135,15 @@
   </si>
   <si>
     <t>2-3, 2-1</t>
+  </si>
+  <si>
+    <t>Ersetzen der Jumperkabeln mit Drahtbrücken, Anlöten der Verbindungsdrähte für einen Infrarot-Sensor, Erste Inbetriebnahme eines Infrarotsensor, erste Ansteuerung mittels PWM der Motoren</t>
+  </si>
+  <si>
+    <t>2-4, 3-1, 3-2, 3-4</t>
+  </si>
+  <si>
+    <t>100%, 30%, 50%, 80%</t>
   </si>
 </sst>
 </file>
@@ -1867,12 +1876,42 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1881,36 +1920,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2421,14 +2430,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="127" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2477,10 +2486,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="117" t="s">
+      <c r="E7" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="117"/>
+      <c r="F7" s="122"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2491,8 +2500,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2503,8 +2512,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2515,8 +2524,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2527,8 +2536,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="121"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2549,49 +2558,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="122"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
+      <c r="B15" s="125"/>
+      <c r="C15" s="125"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="125"/>
+      <c r="F15" s="125"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="128"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2604,64 +2613,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="129"/>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="121"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="117" t="s">
+      <c r="A26" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="117" t="s">
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="117"/>
-      <c r="F26" s="117"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="125" t="s">
+      <c r="A27" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="125"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="130"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="130"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="124" t="s">
+      <c r="A28" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="124"/>
-      <c r="C28" s="124"/>
-      <c r="D28" s="125" t="s">
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="117" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="126" t="s">
+      <c r="A29" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="126"/>
-      <c r="C29" s="126"/>
-      <c r="D29" s="127"/>
-      <c r="E29" s="127"/>
-      <c r="F29" s="127"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2672,16 +2691,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2755,11 +2764,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="131" t="s">
@@ -3576,8 +3585,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,16 +3600,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="127" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5796,7 +5805,7 @@
   <dimension ref="A1:AMO33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6043,14 +6052,28 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="105"/>
+    <row r="12" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="111">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="D12" s="111">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="E12" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="105" t="s">
+        <v>235</v>
+      </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update der AZE in project_overview.xlsx
</commit_message>
<xml_diff>
--- a/project_overview.xlsx
+++ b/project_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023-2024\ESY\self_driving_car\reposi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E72D9B9-E2E4-454E-A507-3FAE298D956F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5483939-7AA2-45B5-A964-B98B579DACBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="240">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1144,6 +1144,18 @@
   </si>
   <si>
     <t>100%, 30%, 50%, 80%</t>
+  </si>
+  <si>
+    <t>Zusammenschrauben der Oberen und unteren Hälfte vom Chasie</t>
+  </si>
+  <si>
+    <t>Reperatur der aufhängung des Sensors mit Heißkleber</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>Ausfüllen der AZE und hochladen auf git</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1549,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1870,11 +1882,32 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1894,33 +1927,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1944,6 +1953,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2430,14 +2454,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="115" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2486,10 +2510,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="122" t="s">
+      <c r="E7" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="122"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2500,8 +2524,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2512,8 +2536,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2524,8 +2548,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2536,8 +2560,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="124"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2558,49 +2582,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="126"/>
-      <c r="C16" s="126"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="122"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="126"/>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="122"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="126"/>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="122"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="120"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
+      <c r="B19" s="127"/>
+      <c r="C19" s="127"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="127"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2613,74 +2637,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="121"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="122" t="s">
+      <c r="A26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="122"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="129"/>
+      <c r="F27" s="129"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117" t="s">
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="124" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
+      <c r="E28" s="124"/>
+      <c r="F28" s="124"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="118"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
+      <c r="B29" s="125"/>
+      <c r="C29" s="125"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2691,6 +2705,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2764,29 +2788,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="131"/>
+      <c r="C3" s="130"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="131"/>
+      <c r="C4" s="130"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="131"/>
+      <c r="C5" s="130"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3009,11 +3033,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3021,18 +3045,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="132" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="134" t="s">
+      <c r="A4" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -3300,14 +3324,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3600,16 +3624,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="115" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4242,19 +4266,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="134" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -4918,16 +4942,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -5703,71 +5727,71 @@
       <c r="A21" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="137" t="s">
+      <c r="B21" s="136" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="137" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="138" t="s">
+      <c r="B23" s="137" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="137" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="136"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="136"/>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="135"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="136"/>
-      <c r="C28" s="136"/>
-      <c r="D28" s="136"/>
+      <c r="B28" s="135"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="136"/>
-      <c r="C29" s="136"/>
-      <c r="D29" s="136"/>
+      <c r="B29" s="135"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5804,8 +5828,8 @@
   </sheetPr>
   <dimension ref="A1:AMO33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5814,23 +5838,23 @@
     <col min="2" max="2" width="8.140625" style="35" customWidth="1"/>
     <col min="3" max="4" width="8.140625" style="108" customWidth="1"/>
     <col min="5" max="5" width="61.5703125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="92" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="141" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="35" customWidth="1"/>
     <col min="9" max="1029" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="131" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5874,13 +5898,13 @@
       <c r="E4" s="107" t="s">
         <v>220</v>
       </c>
-      <c r="F4" s="114" t="s">
+      <c r="F4" s="140" t="s">
         <v>227</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="G4" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="102"/>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
@@ -5898,13 +5922,13 @@
       <c r="E5" s="105" t="s">
         <v>221</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="139" t="s">
         <v>228</v>
       </c>
-      <c r="G5" s="115">
+      <c r="G5" s="138">
         <v>0.7</v>
       </c>
-      <c r="H5" s="85"/>
+      <c r="H5" s="139"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
@@ -5924,13 +5948,13 @@
       <c r="E6" s="105" t="s">
         <v>222</v>
       </c>
-      <c r="F6" s="85" t="s">
+      <c r="F6" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="139" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5950,13 +5974,13 @@
       <c r="E7" s="105" t="s">
         <v>223</v>
       </c>
-      <c r="F7" s="85" t="s">
+      <c r="F7" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
@@ -5974,13 +5998,13 @@
       <c r="E8" s="105" t="s">
         <v>224</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="105" t="s">
+      <c r="G8" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
@@ -5998,11 +6022,11 @@
       <c r="E9" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="139" t="s">
         <v>232</v>
       </c>
-      <c r="G9" s="105"/>
-      <c r="H9" s="2"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
@@ -6020,13 +6044,13 @@
       <c r="E10" s="105" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="85" t="s">
+      <c r="F10" s="139" t="s">
         <v>230</v>
       </c>
-      <c r="G10" s="115" t="s">
+      <c r="G10" s="138" t="s">
         <v>231</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
@@ -6044,13 +6068,13 @@
       <c r="E11" s="105" t="s">
         <v>226</v>
       </c>
-      <c r="F11" s="85" t="s">
+      <c r="F11" s="139" t="s">
         <v>227</v>
       </c>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
@@ -6068,52 +6092,93 @@
       <c r="E12" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="F12" s="85" t="s">
+      <c r="F12" s="139" t="s">
         <v>234</v>
       </c>
-      <c r="G12" s="105" t="s">
+      <c r="G12" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="40">
+        <v>45248</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="111">
+        <v>0.58472222222222225</v>
+      </c>
+      <c r="D13" s="111">
+        <v>0.59861111111111109</v>
+      </c>
+      <c r="E13" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="139" t="s">
+        <v>228</v>
+      </c>
+      <c r="G13" s="138">
+        <v>1</v>
+      </c>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="2"/>
+      <c r="A14" s="40">
+        <v>45248</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" s="111">
+        <v>0.59861111111111109</v>
+      </c>
+      <c r="D14" s="111">
+        <v>0.66805555555555562</v>
+      </c>
+      <c r="E14" s="114" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="139" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" s="138">
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="2"/>
+      <c r="A15" s="40">
+        <v>45248</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" s="111">
+        <v>0.66805555555555562</v>
+      </c>
+      <c r="D15" s="111">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E15" s="114" t="s">
+        <v>239</v>
+      </c>
+      <c r="F15" s="139" t="s">
+        <v>227</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="41"/>
       <c r="C16" s="111"/>
       <c r="D16" s="111"/>
       <c r="E16" s="105"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -6121,9 +6186,9 @@
       <c r="C17" s="111"/>
       <c r="D17" s="111"/>
       <c r="E17" s="105"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
@@ -6131,9 +6196,9 @@
       <c r="C18" s="111"/>
       <c r="D18" s="111"/>
       <c r="E18" s="105"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
@@ -6141,9 +6206,9 @@
       <c r="C19" s="111"/>
       <c r="D19" s="111"/>
       <c r="E19" s="105"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="2"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
@@ -6151,9 +6216,9 @@
       <c r="C20" s="111"/>
       <c r="D20" s="111"/>
       <c r="E20" s="105"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="2"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
@@ -6161,9 +6226,9 @@
       <c r="C21" s="111"/>
       <c r="D21" s="111"/>
       <c r="E21" s="105"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="2"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
@@ -6171,9 +6236,9 @@
       <c r="C22" s="111"/>
       <c r="D22" s="111"/>
       <c r="E22" s="105"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="2"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
@@ -6181,9 +6246,9 @@
       <c r="C23" s="111"/>
       <c r="D23" s="111"/>
       <c r="E23" s="105"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="2"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
@@ -6191,9 +6256,9 @@
       <c r="C24" s="111"/>
       <c r="D24" s="111"/>
       <c r="E24" s="105"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="2"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>
@@ -6201,9 +6266,9 @@
       <c r="C25" s="111"/>
       <c r="D25" s="111"/>
       <c r="E25" s="105"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="2"/>
+      <c r="F25" s="139"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
@@ -6211,9 +6276,9 @@
       <c r="C26" s="111"/>
       <c r="D26" s="111"/>
       <c r="E26" s="105"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="2"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
@@ -6221,9 +6286,9 @@
       <c r="C27" s="111"/>
       <c r="D27" s="111"/>
       <c r="E27" s="105"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="2"/>
+      <c r="F27" s="139"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
@@ -6231,9 +6296,9 @@
       <c r="C28" s="111"/>
       <c r="D28" s="111"/>
       <c r="E28" s="105"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="105"/>
-      <c r="H28" s="2"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
@@ -6241,9 +6306,9 @@
       <c r="C29" s="111"/>
       <c r="D29" s="111"/>
       <c r="E29" s="105"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="2"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
@@ -6251,9 +6316,9 @@
       <c r="C30" s="111"/>
       <c r="D30" s="111"/>
       <c r="E30" s="105"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="105"/>
-      <c r="H30" s="2"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
@@ -6261,9 +6326,9 @@
       <c r="C31" s="111"/>
       <c r="D31" s="111"/>
       <c r="E31" s="105"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="105"/>
-      <c r="H31" s="2"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
@@ -6271,9 +6336,9 @@
       <c r="C32" s="111"/>
       <c r="D32" s="111"/>
       <c r="E32" s="105"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="105"/>
-      <c r="H32" s="2"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
@@ -6281,9 +6346,9 @@
       <c r="C33" s="112"/>
       <c r="D33" s="112"/>
       <c r="E33" s="106"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="106"/>
-      <c r="H33" s="24"/>
+      <c r="F33" s="142"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>